<commit_message>
ajustando script para procesar solo titulo
</commit_message>
<xml_diff>
--- a/Ecopetrol OHLCV+indicadores.xlsx
+++ b/Ecopetrol OHLCV+indicadores.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11496" windowHeight="7308"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="11496" windowHeight="7308"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -53,7 +53,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -67,6 +67,7 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -120,7 +121,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -428,14 +429,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I1705"/>
+  <dimension ref="A1:I1706"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J26" sqref="J26"/>
+      <selection activeCell="I16" sqref="I16:I1706"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="21.5546875" customWidth="1"/>
     <col min="7" max="7" width="10.21875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -49758,6 +49760,11 @@
         <v>61.089226263439514</v>
       </c>
     </row>
+    <row r="1706" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H1706">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>